<commit_message>
update result data Zeeland
</commit_message>
<xml_diff>
--- a/Plotting/result_data_long_Zeeland.xlsx
+++ b/Plotting/result_data_long_Zeeland.xlsx
@@ -563,17 +563,17 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Z:\AdOpt_NET0\AdOpt_results\MY\EmissionLimit Brownfield\Zeeland\20250415091828_2030_minC_DD10-1\optimization_results.h5</t>
+          <t>Z:\AdOpt_NET0\AdOpt_results\MY\EmissionLimit Brownfield\Zeeland\20250428094955_2030_minC_DD10-1\optimization_results.h5</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Z:\AdOpt_NET0\AdOpt_results\MY\EmissionLimit Brownfield\Zeeland\20250422100226_2040_minC_DD10-1\optimization_results.h5</t>
+          <t>Z:\AdOpt_NET0\AdOpt_results\MY\EmissionLimit Brownfield\Zeeland\20250428122724_2040_minC_DD10-1\optimization_results.h5</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Z:\AdOpt_NET0\AdOpt_results\MY\EmissionLimit Brownfield\Zeeland\20250422232409_2050_minC_DD10-1\optimization_results.h5</t>
+          <t>Z:\AdOpt_NET0\AdOpt_results\MY\EmissionLimit Brownfield\Zeeland\20250501121718_2050_minC_DD10-1\optimization_results.h5</t>
         </is>
       </c>
     </row>
@@ -593,13 +593,13 @@
         <v>4094571776.672101</v>
       </c>
       <c r="E6" t="n">
-        <v>6460664590.957397</v>
+        <v>6377673518.162631</v>
       </c>
       <c r="F6" t="n">
-        <v>5460087660.276251</v>
+        <v>5450814552.258259</v>
       </c>
       <c r="G6" t="n">
-        <v>3762519842.796689</v>
+        <v>3760890499.657729</v>
       </c>
     </row>
     <row r="7">
@@ -613,10 +613,10 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>633481140.7637757</v>
+        <v>537546119.7996608</v>
       </c>
       <c r="G7" t="n">
-        <v>970017361.7419047</v>
+        <v>875326557.1320901</v>
       </c>
     </row>
     <row r="8">
@@ -629,13 +629,13 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
-        <v>6460664590.957397</v>
+        <v>6377673518.162631</v>
       </c>
       <c r="F8" t="n">
-        <v>6093568801.040027</v>
+        <v>5988360672.05792</v>
       </c>
       <c r="G8" t="n">
-        <v>4732537204.538593</v>
+        <v>4636217056.78982</v>
       </c>
     </row>
     <row r="9">
@@ -656,7 +656,7 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
-        <v>166532894557.7224</v>
+        <v>164647051272.1071</v>
       </c>
     </row>
     <row r="10">
@@ -675,13 +675,13 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>1285836.673440453</v>
+        <v>1308190.96367628</v>
       </c>
       <c r="F10" t="n">
-        <v>642918.3364999938</v>
+        <v>654095.4818381065</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.769512891769409e-08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -700,7 +700,7 @@
         <v>555.9053021890891</v>
       </c>
       <c r="E11" t="n">
-        <v>941.2704836930354</v>
+        <v>894.6947646023427</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -725,10 +725,10 @@
         <v>43.02380952380953</v>
       </c>
       <c r="E12" t="n">
-        <v>46.10831550588128</v>
+        <v>43.368</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1.496635535656232</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -750,13 +750,13 @@
         <v>557.7582217835803</v>
       </c>
       <c r="E13" t="n">
-        <v>381.3882019773707</v>
+        <v>383.0596234757299</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>6.767893059495433</v>
       </c>
       <c r="G13" t="n">
-        <v>167.401609169428</v>
+        <v>155.5646101381337</v>
       </c>
     </row>
     <row r="14">
@@ -775,7 +775,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>501.082937427457</v>
+        <v>502.5368929636838</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -803,10 +803,10 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>200.5916802758914</v>
+        <v>210.605109753033</v>
       </c>
       <c r="G15" t="n">
-        <v>156.2498832117323</v>
+        <v>142.9572210309153</v>
       </c>
     </row>
     <row r="16">
@@ -919,10 +919,10 @@
         <v>951.3414652600432</v>
       </c>
       <c r="E20" t="n">
-        <v>753.0747362557166</v>
+        <v>894.9482235336452</v>
       </c>
       <c r="F20" t="n">
-        <v>176.5415435645167</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
@@ -944,10 +944,10 @@
         <v>1238.095238095238</v>
       </c>
       <c r="E21" t="n">
-        <v>1326.858000169245</v>
+        <v>1248</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>43.06864850809301</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
@@ -969,10 +969,10 @@
         <v>1238.095238095238</v>
       </c>
       <c r="E22" t="n">
-        <v>1326.858000169245</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>43.06864850809301</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
@@ -994,7 +994,7 @@
         <v>299.414963165223</v>
       </c>
       <c r="E23" t="n">
-        <v>469.0000000000001</v>
+        <v>469</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -1019,7 +1019,7 @@
         <v>440.1399958528778</v>
       </c>
       <c r="E24" t="n">
-        <v>689.4299999999986</v>
+        <v>689.4300000000668</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -1088,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>88.3200931315484</v>
+        <v>88.3200931315462</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -1182,10 +1182,10 @@
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>16753.82088623411</v>
+        <v>5113.471999999979</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>10714.65279238021</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
@@ -1207,7 +1207,7 @@
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>1474.47323103563</v>
+        <v>1581.396712910418</v>
       </c>
       <c r="F32" t="n">
         <v>4065</v>
@@ -1232,10 +1232,10 @@
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>214.4220172874399</v>
+        <v>182.3734825774716</v>
       </c>
       <c r="F33" t="n">
-        <v>1134.881231233874</v>
+        <v>1331.889642902058</v>
       </c>
       <c r="G33" t="n">
         <v>0</v>
@@ -1257,10 +1257,10 @@
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>2.700062395888381e-11</v>
+        <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>943.9042714094785</v>
+        <v>5724.855129380961</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
@@ -1282,10 +1282,10 @@
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>912.3603805359496</v>
+        <v>1715.087259231281</v>
       </c>
       <c r="F35" t="n">
-        <v>13633.48029136625</v>
+        <v>13841.18942943548</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
@@ -1307,10 +1307,10 @@
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>-7.161172487738074e-11</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>8507.366129941622</v>
+        <v>3790.473682560014</v>
       </c>
       <c r="G36" t="n">
         <v>0</v>
@@ -1332,10 +1332,10 @@
         <v>177.9008540036281</v>
       </c>
       <c r="E37" t="n">
-        <v>140.824975679819</v>
+        <v>167.3553178007917</v>
       </c>
       <c r="F37" t="n">
-        <v>33.01326864656463</v>
+        <v>0</v>
       </c>
       <c r="G37" t="n">
         <v>0</v>
@@ -1357,7 +1357,7 @@
         <v>951.3414652600432</v>
       </c>
       <c r="E38" t="n">
-        <v>1254.157673683174</v>
+        <v>1350.322154607045</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
@@ -1457,13 +1457,13 @@
         <v>190.2682930520829</v>
       </c>
       <c r="E42" t="n">
-        <v>263.0905160946049</v>
+        <v>259.6151598489242</v>
       </c>
       <c r="F42" t="n">
-        <v>354</v>
+        <v>242.9559191542486</v>
       </c>
       <c r="G42" t="n">
-        <v>397.755844417374</v>
+        <v>407.3118751406292</v>
       </c>
     </row>
     <row r="43">
@@ -1482,10 +1482,10 @@
         <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>1.184369679440014e-11</v>
+        <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
+        <v>2.816591404553037e-11</v>
       </c>
       <c r="G43" t="n">
         <v>0</v>
@@ -1635,7 +1635,7 @@
         <v>469</v>
       </c>
       <c r="F49" t="n">
-        <v>469</v>
+        <v>469.0000000000455</v>
       </c>
       <c r="G49" t="n">
         <v>469</v>
@@ -1835,10 +1835,10 @@
         <v>1900</v>
       </c>
       <c r="F57" t="n">
-        <v>3250</v>
+        <v>3250.00000000464</v>
       </c>
       <c r="G57" t="n">
-        <v>4600.000000009787</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="58">
@@ -2057,13 +2057,13 @@
         <v>90.61256425745759</v>
       </c>
       <c r="E66" t="n">
-        <v>153.4270888419648</v>
+        <v>145.8352466307604</v>
       </c>
       <c r="F66" t="n">
-        <v>153.4270888419648</v>
+        <v>145.8352466301818</v>
       </c>
       <c r="G66" t="n">
-        <v>132.587190975594</v>
+        <v>145.8352466301818</v>
       </c>
     </row>
     <row r="67">
@@ -2132,13 +2132,13 @@
         <v>951.3414652602287</v>
       </c>
       <c r="E69" t="n">
-        <v>1254.157673683174</v>
+        <v>1350.322154607045</v>
       </c>
       <c r="F69" t="n">
-        <v>1196.458970246627</v>
+        <v>1210.649120408641</v>
       </c>
       <c r="G69" t="n">
-        <v>929.6162798202333</v>
+        <v>894.9482235336452</v>
       </c>
     </row>
     <row r="70">
@@ -2410,7 +2410,7 @@
         <v>0</v>
       </c>
       <c r="F80" t="n">
-        <v>0</v>
+        <v>6.084022174945858e-14</v>
       </c>
       <c r="G80" t="n">
         <v>0</v>
@@ -2507,13 +2507,13 @@
         <v>135.6201043124598</v>
       </c>
       <c r="E84" t="n">
-        <v>196.8242051959786</v>
+        <v>186.5220559262779</v>
       </c>
       <c r="F84" t="n">
-        <v>196.8242051959786</v>
+        <v>188.3584277279992</v>
       </c>
       <c r="G84" t="n">
-        <v>174.6490532076666</v>
+        <v>186.7105215149341</v>
       </c>
     </row>
     <row r="85">
@@ -2532,7 +2532,7 @@
         <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>88.32009313182347</v>
+        <v>88.32009313296318</v>
       </c>
       <c r="F85" t="n">
         <v>0</v>
@@ -2781,10 +2781,10 @@
       </c>
       <c r="E95" t="inlineStr"/>
       <c r="F95" t="n">
-        <v>147.5567893742756</v>
+        <v>146.2075946034622</v>
       </c>
       <c r="G95" t="n">
-        <v>109.8290814684159</v>
+        <v>107.9031888874626</v>
       </c>
     </row>
     <row r="96">
@@ -2833,13 +2833,13 @@
       <c r="C98" t="inlineStr"/>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="n">
-        <v>0</v>
+        <v>1248</v>
       </c>
       <c r="F98" t="n">
-        <v>1326.858000169245</v>
+        <v>1248</v>
       </c>
       <c r="G98" t="n">
-        <v>1326.858000169245</v>
+        <v>1291.068648508093</v>
       </c>
     </row>
     <row r="99">
@@ -2883,10 +2883,10 @@
       <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr"/>
       <c r="F101" t="n">
-        <v>941.2704836930354</v>
+        <v>894.6947646023427</v>
       </c>
       <c r="G101" t="n">
-        <v>941.2704836930354</v>
+        <v>894.6947646023427</v>
       </c>
     </row>
     <row r="102">
@@ -2900,10 +2900,10 @@
       <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr"/>
       <c r="F102" t="n">
-        <v>46.10831550588128</v>
+        <v>43.368</v>
       </c>
       <c r="G102" t="n">
-        <v>46.10831550588128</v>
+        <v>44.86463553565623</v>
       </c>
     </row>
     <row r="103">
@@ -2917,10 +2917,10 @@
       <c r="D103" t="inlineStr"/>
       <c r="E103" t="inlineStr"/>
       <c r="F103" t="n">
-        <v>381.3882019773707</v>
+        <v>383.0596234757299</v>
       </c>
       <c r="G103" t="n">
-        <v>381.3882019773707</v>
+        <v>389.8275165352254</v>
       </c>
     </row>
     <row r="104">
@@ -2934,10 +2934,10 @@
       <c r="D104" t="inlineStr"/>
       <c r="E104" t="inlineStr"/>
       <c r="F104" t="n">
-        <v>501.082937427457</v>
+        <v>502.5368929636838</v>
       </c>
       <c r="G104" t="n">
-        <v>501.082937427457</v>
+        <v>502.5368929636838</v>
       </c>
     </row>
     <row r="105">
@@ -2951,10 +2951,10 @@
       <c r="D105" t="inlineStr"/>
       <c r="E105" t="inlineStr"/>
       <c r="F105" t="n">
-        <v>753.0747362557166</v>
+        <v>894.9482235336452</v>
       </c>
       <c r="G105" t="n">
-        <v>929.6162798202333</v>
+        <v>894.9482235336452</v>
       </c>
     </row>
     <row r="106">
@@ -2968,10 +2968,10 @@
       <c r="D106" t="inlineStr"/>
       <c r="E106" t="inlineStr"/>
       <c r="F106" t="n">
-        <v>1326.858000169245</v>
+        <v>1248</v>
       </c>
       <c r="G106" t="n">
-        <v>1326.858000169245</v>
+        <v>1291.068648508093</v>
       </c>
     </row>
     <row r="107">
@@ -2985,10 +2985,10 @@
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr"/>
       <c r="F107" t="n">
-        <v>469.0000000000001</v>
+        <v>469</v>
       </c>
       <c r="G107" t="n">
-        <v>469.0000000000001</v>
+        <v>469</v>
       </c>
     </row>
     <row r="108">
@@ -3002,10 +3002,10 @@
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr"/>
       <c r="F108" t="n">
-        <v>689.4299999999986</v>
+        <v>689.4300000000668</v>
       </c>
       <c r="G108" t="n">
-        <v>689.4299999999986</v>
+        <v>689.4300000000668</v>
       </c>
     </row>
     <row r="109">
@@ -3019,10 +3019,10 @@
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr"/>
       <c r="F109" t="n">
-        <v>88.3200931315484</v>
+        <v>88.3200931315462</v>
       </c>
       <c r="G109" t="n">
-        <v>88.3200931315484</v>
+        <v>88.3200931315462</v>
       </c>
     </row>
     <row r="110">
@@ -3053,10 +3053,10 @@
       <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr"/>
       <c r="F111" t="n">
-        <v>16753.82088623411</v>
+        <v>5113.471999999979</v>
       </c>
       <c r="G111" t="n">
-        <v>16753.82088623411</v>
+        <v>15828.12479238019</v>
       </c>
     </row>
     <row r="112">
@@ -3070,10 +3070,10 @@
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr"/>
       <c r="F112" t="n">
-        <v>1474.47323103563</v>
+        <v>1581.396712910418</v>
       </c>
       <c r="G112" t="n">
-        <v>5539.47323103563</v>
+        <v>5646.396712910419</v>
       </c>
     </row>
     <row r="113">
@@ -3087,16 +3087,16 @@
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr"/>
       <c r="F113" t="n">
-        <v>214.4220172874399</v>
+        <v>182.3734825774716</v>
       </c>
       <c r="G113" t="n">
-        <v>1349.303248521314</v>
+        <v>1514.26312547953</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>size_Storage_Ethylene_existing</t>
+          <t>size_Storage_H2_existing</t>
         </is>
       </c>
       <c r="B114" t="inlineStr"/>
@@ -3104,16 +3104,16 @@
       <c r="D114" t="inlineStr"/>
       <c r="E114" t="inlineStr"/>
       <c r="F114" t="n">
-        <v>2.700062395888381e-11</v>
+        <v>1715.087259231281</v>
       </c>
       <c r="G114" t="n">
-        <v>943.9042714095056</v>
+        <v>15556.27668866676</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>size_Storage_H2_existing</t>
+          <t>size_WGS_m_existing</t>
         </is>
       </c>
       <c r="B115" t="inlineStr"/>
@@ -3121,16 +3121,16 @@
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr"/>
       <c r="F115" t="n">
-        <v>912.3603805359496</v>
+        <v>167.3553178007917</v>
       </c>
       <c r="G115" t="n">
-        <v>14545.8406719022</v>
+        <v>167.3553178007917</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>size_WGS_m_existing</t>
+          <t>size_feedgas_mixer_existing</t>
         </is>
       </c>
       <c r="B116" t="inlineStr"/>
@@ -3138,33 +3138,31 @@
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr"/>
       <c r="F116" t="n">
-        <v>140.824975679819</v>
+        <v>1350.322154607045</v>
       </c>
       <c r="G116" t="n">
-        <v>173.8382443263836</v>
+        <v>1350.322154607045</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>size_feedgas_mixer_existing</t>
+          <t>size_CO2_mixer_existing</t>
         </is>
       </c>
       <c r="B117" t="inlineStr"/>
       <c r="C117" t="inlineStr"/>
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr"/>
-      <c r="F117" t="n">
-        <v>1254.157673683174</v>
-      </c>
+      <c r="F117" t="inlineStr"/>
       <c r="G117" t="n">
-        <v>1254.157673683174</v>
+        <v>210.605109753033</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>size_CO2_mixer_existing</t>
+          <t>size_CO2electrolysis_existing</t>
         </is>
       </c>
       <c r="B118" t="inlineStr"/>
@@ -3173,13 +3171,13 @@
       <c r="E118" t="inlineStr"/>
       <c r="F118" t="inlineStr"/>
       <c r="G118" t="n">
-        <v>200.5916802758914</v>
+        <v>146.2075946034622</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>size_CO2electrolysis_existing</t>
+          <t>size_Storage_Ethylene_existing</t>
         </is>
       </c>
       <c r="B119" t="inlineStr"/>
@@ -3188,7 +3186,7 @@
       <c r="E119" t="inlineStr"/>
       <c r="F119" t="inlineStr"/>
       <c r="G119" t="n">
-        <v>147.5567893742756</v>
+        <v>5724.855129380961</v>
       </c>
     </row>
     <row r="120">
@@ -3203,7 +3201,7 @@
       <c r="E120" t="inlineStr"/>
       <c r="F120" t="inlineStr"/>
       <c r="G120" t="n">
-        <v>8507.366129941622</v>
+        <v>3790.473682560014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>